<commit_message>
Downloaded new data for homework assignment and class project
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/SOC5670_Homework01_DataDictionary.xlsx
+++ b/Assignments/Homework01/SOC5670_Homework01_DataDictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -38,7 +38,13 @@
     <t>R12443901</t>
   </si>
   <si>
-    <t>Census tract level data from Social Explorer for Illinois and Missouri.  ACS 2018 (5-year estimates) for tables A00001, A00002, A00003, A02001, A01001, A02001, A04001, A12001, B17008, A17009.</t>
+    <t>SocialExplorer.com data for all census tracts in Missouri.  ACS 2018 (5-year estimates) for tables A02001, A01001, A04001, A14028, A12001, A12002, B17008, A14001, A10016, A13003A, A13003B, A13003C, A09001, B09001. Dollar values inflation adjusted to 2018 dollars.</t>
+  </si>
+  <si>
+    <t>R12459585</t>
+  </si>
+  <si>
+    <t>SocialExplorer.com census tract level data for Illinois and Missouri.  ACS 2018 (5-year estimates) for tables A00001, A00002, A00003, A02001, A01001, A02001, A04001, A12001, B17008, A17009.</t>
   </si>
 </sst>
 </file>
@@ -419,11 +425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,6 +459,17 @@
         <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>43877</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>